<commit_message>
Only write thickness to excel if value is greater than 0
</commit_message>
<xml_diff>
--- a/ExportDXF/Templates/BomTemplate.xlsx
+++ b/ExportDXF/Templates/BomTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aj.REMCO\Source\Repos\ExportDXF\ExportDXF\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{369855F2-DDB0-438F-896F-1AE6E40A3063}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{11CA7B5F-8F8E-41B7-834D-A219B5EEDB96}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11625" xr2:uid="{97300FE0-786B-4DD8-9D4E-FAA72609135B}"/>
   </bookViews>
@@ -102,7 +102,28 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -414,7 +435,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F79AB71B-87A5-4BED-85D3-9FDFBDDB7EC0}">
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -422,7 +445,7 @@
     <col min="2" max="2" width="13" style="3" customWidth="1"/>
     <col min="3" max="3" width="53.140625" style="1" customWidth="1"/>
     <col min="4" max="4" width="43.85546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" style="3" customWidth="1"/>
     <col min="6" max="6" width="27.85546875" style="1" customWidth="1"/>
     <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>

</xml_diff>

<commit_message>
Include kfactor in BOM
</commit_message>
<xml_diff>
--- a/ExportDXF/Templates/BomTemplate.xlsx
+++ b/ExportDXF/Templates/BomTemplate.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aj.REMCO\Source\Repos\ExportDXF\ExportDXF\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{11CA7B5F-8F8E-41B7-834D-A219B5EEDB96}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{B2778D31-4C21-404C-BF09-050168BE9C23}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11625" xr2:uid="{97300FE0-786B-4DD8-9D4E-FAA72609135B}"/>
   </bookViews>
   <sheets>
     <sheet name="Parts" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Parts!$A$1:$F$1</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Item #</t>
   </si>
@@ -43,6 +46,9 @@
   </si>
   <si>
     <t>Part</t>
+  </si>
+  <si>
+    <t>K-Factor</t>
   </si>
 </sst>
 </file>
@@ -102,28 +108,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -433,11 +418,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F79AB71B-87A5-4BED-85D3-9FDFBDDB7EC0}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -450,7 +433,7 @@
     <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -469,8 +452,12 @@
       <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:F1" xr:uid="{EF02C8F9-45EE-4643-9391-B20941B55CC7}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Include bend radius on BOM
</commit_message>
<xml_diff>
--- a/ExportDXF/Templates/BomTemplate.xlsx
+++ b/ExportDXF/Templates/BomTemplate.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aj.REMCO\Source\Repos\ExportDXF\ExportDXF\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aj.REMCO\Desktop\ExportDXF\ExportDXF\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{B2778D31-4C21-404C-BF09-050168BE9C23}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{37313F72-1745-416C-AF4C-5B67AEA0E1A2}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11625" xr2:uid="{97300FE0-786B-4DD8-9D4E-FAA72609135B}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Item #</t>
   </si>
@@ -49,6 +49,9 @@
   </si>
   <si>
     <t>K-Factor</t>
+  </si>
+  <si>
+    <t>Default Bend Radius</t>
   </si>
 </sst>
 </file>
@@ -418,22 +421,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F79AB71B-87A5-4BED-85D3-9FDFBDDB7EC0}">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13" style="3" customWidth="1"/>
+    <col min="2" max="2" width="10" style="3" customWidth="1"/>
     <col min="3" max="3" width="53.140625" style="1" customWidth="1"/>
     <col min="4" max="4" width="43.85546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="16.140625" style="3" customWidth="1"/>
     <col min="6" max="6" width="27.85546875" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="1"/>
+    <col min="7" max="7" width="9.85546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="22.140625" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -454,6 +461,9 @@
       </c>
       <c r="G1" s="2" t="s">
         <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Save file name in excel file.
</commit_message>
<xml_diff>
--- a/ExportDXF/Templates/BomTemplate.xlsx
+++ b/ExportDXF/Templates/BomTemplate.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aj.REMCO\Desktop\ExportDXF\ExportDXF\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aisaa\Desktop\ExportDXF\ExportDXF\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{37313F72-1745-416C-AF4C-5B67AEA0E1A2}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{E6216284-6003-44A6-BC76-F828F531DC1B}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11625" xr2:uid="{97300FE0-786B-4DD8-9D4E-FAA72609135B}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Parts" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Parts!$A$1:$F$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Parts!$A$1:$G$1</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Item #</t>
   </si>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t>Default Bend Radius</t>
+  </si>
+  <si>
+    <t>File Name</t>
   </si>
 </sst>
 </file>
@@ -421,53 +424,54 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F79AB71B-87A5-4BED-85D3-9FDFBDDB7EC0}">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10" style="3" customWidth="1"/>
-    <col min="3" max="3" width="53.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="43.85546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="27.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="9.85546875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="22.140625" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="2" width="16.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10" style="3" customWidth="1"/>
+    <col min="4" max="4" width="53.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="43.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="27.85546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="9.85546875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="22.140625" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F1" xr:uid="{EF02C8F9-45EE-4643-9391-B20941B55CC7}"/>
+  <autoFilter ref="A1:G1" xr:uid="{EF02C8F9-45EE-4643-9391-B20941B55CC7}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Improved excel BOM template for printing.
</commit_message>
<xml_diff>
--- a/ExportDXF/Templates/BomTemplate.xlsx
+++ b/ExportDXF/Templates/BomTemplate.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aisaa\Desktop\ExportDXF\ExportDXF\Templates\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{E6216284-6003-44A6-BC76-F828F531DC1B}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11625" xr2:uid="{97300FE0-786B-4DD8-9D4E-FAA72609135B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11625"/>
   </bookViews>
   <sheets>
     <sheet name="Parts" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Parts!$A$1:$G$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Parts!$A$1:$I$1</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -60,8 +54,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -87,7 +81,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -95,11 +89,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -107,8 +116,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -170,7 +191,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -222,7 +243,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -416,63 +437,70 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F79AB71B-87A5-4BED-85D3-9FDFBDDB7EC0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="16.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10" style="3" customWidth="1"/>
-    <col min="4" max="4" width="53.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="43.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="16.140625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="27.85546875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="9.85546875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="22.140625" style="1" customWidth="1"/>
+    <col min="1" max="2" width="16.140625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="10" style="6" customWidth="1"/>
+    <col min="4" max="4" width="53.140625" style="7" customWidth="1"/>
+    <col min="5" max="5" width="43.85546875" style="5" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" style="6" customWidth="1"/>
+    <col min="7" max="7" width="27.85546875" style="5" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" style="5" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" style="5" customWidth="1"/>
     <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:9" s="2" customFormat="1" ht="34.5" customHeight="1">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="4" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G1" xr:uid="{EF02C8F9-45EE-4643-9391-B20941B55CC7}"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <autoFilter ref="A1:I1"/>
+  <pageMargins left="0.2" right="0.2" top="0.6" bottom="0.6" header="0.3" footer="0.2"/>
+  <pageSetup scale="62" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"-,Bold"&amp;14BILL OF MATERIALS&amp;R&amp;D &amp;T</oddHeader>
+    <oddFooter>&amp;L&amp;Z&amp;F</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Print column headers on all pages of BOM
</commit_message>
<xml_diff>
--- a/ExportDXF/Templates/BomTemplate.xlsx
+++ b/ExportDXF/Templates/BomTemplate.xlsx
@@ -11,6 +11,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Parts!$A$1:$I$1</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">Parts!$1:$1</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
@@ -437,7 +438,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -497,7 +498,7 @@
   </sheetData>
   <autoFilter ref="A1:I1"/>
   <pageMargins left="0.2" right="0.2" top="0.6" bottom="0.6" header="0.3" footer="0.2"/>
-  <pageSetup scale="62" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup scale="64" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"-,Bold"&amp;14BILL OF MATERIALS&amp;R&amp;D &amp;T</oddHeader>
     <oddFooter>&amp;L&amp;Z&amp;F</oddFooter>

</xml_diff>

<commit_message>
Extract referenced configuration name with part.
</commit_message>
<xml_diff>
--- a/ExportDXF/Templates/BomTemplate.xlsx
+++ b/ExportDXF/Templates/BomTemplate.xlsx
@@ -10,10 +10,10 @@
     <sheet name="Parts" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Parts!$A$1:$I$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Parts!$A$1:$J$1</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Parts!$1:$1</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="125725"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
     <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Item #</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t>File Name</t>
+  </si>
+  <si>
+    <t>Configuration</t>
   </si>
 </sst>
 </file>
@@ -438,7 +441,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -449,24 +452,28 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="16.140625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="10" style="6" customWidth="1"/>
-    <col min="4" max="4" width="53.140625" style="7" customWidth="1"/>
-    <col min="5" max="5" width="43.85546875" style="5" customWidth="1"/>
-    <col min="6" max="6" width="16.140625" style="6" customWidth="1"/>
-    <col min="7" max="7" width="27.85546875" style="5" customWidth="1"/>
-    <col min="8" max="8" width="13.140625" style="5" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" style="5" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.5703125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="26.42578125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="7.85546875" style="6" customWidth="1"/>
+    <col min="4" max="4" width="45" style="7" customWidth="1"/>
+    <col min="5" max="5" width="40.5703125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" style="6" customWidth="1"/>
+    <col min="8" max="8" width="23.7109375" style="5" customWidth="1"/>
+    <col min="9" max="9" width="10" style="5" customWidth="1"/>
+    <col min="10" max="10" width="13.42578125" style="5" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" ht="34.5" customHeight="1">
+    <row r="1" spans="1:10" s="2" customFormat="1" ht="44.25" customHeight="1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -483,20 +490,25 @@
         <v>5</v>
       </c>
       <c r="F1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I1"/>
+  <autoFilter ref="A1:J1">
+    <filterColumn colId="5"/>
+  </autoFilter>
   <pageMargins left="0.2" right="0.2" top="0.6" bottom="0.6" header="0.3" footer="0.2"/>
   <pageSetup scale="64" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <headerFooter>

</xml_diff>